<commit_message>
Include real EURO cost implication of additional cable
EUROS/km/station still only rough, but numbers are so small that it
seems even the most complex of these layouts is not killed by cable
costs.
</commit_message>
<xml_diff>
--- a/results/iantconfig/Iantconfig_text_results/Antconfig_results_overview.xlsx
+++ b/results/iantconfig/Iantconfig_text_results/Antconfig_results_overview.xlsx
@@ -41,6 +41,7 @@
     <definedName name="model01_cables" localSheetId="1">Overview!$B$30:$C$38</definedName>
     <definedName name="model02_cables" localSheetId="1">Overview!$D$30:$E$38</definedName>
     <definedName name="model03_cables" localSheetId="1">Overview!$F$30:$G$38</definedName>
+    <definedName name="rfonfcost_per_station_per_km">Overview!$H$20</definedName>
     <definedName name="ska1_v5_cables" localSheetId="1">Overview!$B$40:$C$41</definedName>
     <definedName name="ska1v5_snap.20x3" localSheetId="0">'Snapshot setting'!$A$3:$C$23</definedName>
     <definedName name="ska1v5_snap.20x3_1" localSheetId="0">'Snapshot setting'!$A$55:$C$75</definedName>
@@ -83,6 +84,30 @@
           <t xml:space="preserve">
 Mean of ratio between uvgap of altered layout and uvgap of v5 layout.
 Uvgap is calculated for baselines out ot a range of different maximum baselines from 580m to 10km</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Rosie Bolton:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This is a rough number from Nima, we must ask Tom Booler(sp?) for the laterst RFonF costs and consider infrastructure cost implications</t>
         </r>
       </text>
     </comment>
@@ -398,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
   <si>
     <t>baseline</t>
   </si>
@@ -558,6 +583,15 @@
   <si>
     <t>Guess for now - need number</t>
   </si>
+  <si>
+    <t>RF on fibre cost per km per station</t>
+  </si>
+  <si>
+    <t>relative increase</t>
+  </si>
+  <si>
+    <t>Cost increaes (kEUROS)</t>
+  </si>
 </sst>
 </file>
 
@@ -630,7 +664,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -670,14 +704,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -697,6 +738,9 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -716,6 +760,9 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -753,7 +800,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2340,17 +2386,407 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145272792"/>
-        <c:axId val="2104159464"/>
+        <c:axId val="-2078347624"/>
+        <c:axId val="-2078600088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145272792"/>
+        <c:axId val="-2078347624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2078600088"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2078600088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2078347624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>UVGAP</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> ratio as function of cable length</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$B$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Overview!$C$7:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.174186687413501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.047565317308</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9519635450681</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.2948211807921</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.2614668508579</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.0415784670608</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.1491152391404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.3013568910976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>59.7632291219067</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Overview!$B$7:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.970887059894747</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.901928250740241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.842262719639391</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.761651830255601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.681377695741551</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.605407217034242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.549089794972765</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.492312265095318</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.433705016363919</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Overview!$G$7:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.647224457474</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.3587928426985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.002906916146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.7340257677076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.770356736764</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.0167962850801</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>112.3569257895242</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>156.3035340335132</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>214.4748471278922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Overview!$F$7:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.893048804378685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.792734940516993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.715116326820911</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.665349470720177</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.617935077583338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.573176578772192</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.518270317536034</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.495653536573672</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.479320605040263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Overview!$J$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Overview!$K$7:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>4.647224457474</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.3587928426985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.002906916146</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>34.7340257677076</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53.770356736764</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.5504683529669</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.6580051250465</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.8102467770036</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>98.2721190078122</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Overview!$J$7:$J$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.893048804378685</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.792734940516993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.715116326820911</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.665349470720177</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.617935077583338</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.559122877149948</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.507337984103468</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.471205309193636</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.427995345125993</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2146145080"/>
+        <c:axId val="2146140328"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2146145080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>Additional cable length, km (worst case)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2358,19 +2794,40 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104159464"/>
+        <c:crossAx val="2146140328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2104159464"/>
+        <c:axId val="2146140328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:minorGridlines/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>UVGAP</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> ratio</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -2378,7 +2835,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145272792"/>
+        <c:crossAx val="2146145080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2430,7 +2887,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4017,30 +4473,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2145321240"/>
-        <c:axId val="2145338200"/>
+        <c:axId val="-2127323640"/>
+        <c:axId val="-2127068040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2145321240"/>
+        <c:axId val="-2127323640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145338200"/>
+        <c:crossAx val="-2127068040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145338200"/>
+        <c:axId val="-2127068040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4048,21 +4503,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145321240"/>
+        <c:crossAx val="-2127323640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4107,7 +4560,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -5694,30 +6146,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2103942328"/>
-        <c:axId val="2103633688"/>
+        <c:axId val="-2126261880"/>
+        <c:axId val="-2125481928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2103942328"/>
+        <c:axId val="-2126261880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103633688"/>
+        <c:crossAx val="-2125481928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2103633688"/>
+        <c:axId val="-2125481928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5725,21 +6176,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103942328"/>
+        <c:crossAx val="-2126261880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5784,7 +6233,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -7371,30 +7819,29 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080751000"/>
-        <c:axId val="2145070872"/>
+        <c:axId val="-2126739880"/>
+        <c:axId val="-2126121112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080751000"/>
+        <c:axId val="-2126739880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145070872"/>
+        <c:crossAx val="-2126121112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145070872"/>
+        <c:axId val="-2126121112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7402,21 +7849,19 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080751000"/>
+        <c:crossAx val="-2126739880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -9047,11 +9492,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097314344"/>
-        <c:axId val="2097299608"/>
+        <c:axId val="2104908968"/>
+        <c:axId val="-2081383448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097314344"/>
+        <c:axId val="2104908968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9064,12 +9509,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097299608"/>
+        <c:crossAx val="-2081383448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097299608"/>
+        <c:axId val="-2081383448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9083,7 +9528,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097314344"/>
+        <c:crossAx val="2104908968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -10720,11 +11165,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2080708392"/>
-        <c:axId val="2097396088"/>
+        <c:axId val="2085976472"/>
+        <c:axId val="2105173256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2080708392"/>
+        <c:axId val="2085976472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10737,12 +11182,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097396088"/>
+        <c:crossAx val="2105173256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097396088"/>
+        <c:axId val="2105173256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10756,7 +11201,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080708392"/>
+        <c:crossAx val="2085976472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11133,11 +11578,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2085079864"/>
-        <c:axId val="2092539688"/>
+        <c:axId val="2099201960"/>
+        <c:axId val="2145322824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2085079864"/>
+        <c:axId val="2099201960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11171,12 +11616,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2092539688"/>
+        <c:crossAx val="2145322824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2092539688"/>
+        <c:axId val="2145322824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11211,7 +11656,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085079864"/>
+        <c:crossAx val="2099201960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11262,7 +11707,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> ratio as function of cable length</a:t>
+              <a:t> ratio as function of additional RF on F cable cost:</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -11293,7 +11738,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$C$7:$C$15</c:f>
+              <c:f>Overview!$E$7:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11370,7 +11815,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overview!$E$5</c:f>
+              <c:f>Overview!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11381,7 +11826,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$F$7:$F$15</c:f>
+              <c:f>Overview!$G$7:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11417,7 +11862,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overview!$E$7:$E$15</c:f>
+              <c:f>Overview!$F$7:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11458,7 +11903,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overview!$H$5</c:f>
+              <c:f>Overview!$J$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11469,7 +11914,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$I$7:$I$15</c:f>
+              <c:f>Overview!$K$7:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11505,7 +11950,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overview!$H$7:$H$15</c:f>
+              <c:f>Overview!$J$7:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11542,7 +11987,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -11550,11 +11994,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2143420568"/>
-        <c:axId val="2086101656"/>
+        <c:axId val="2085989576"/>
+        <c:axId val="2145085528"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2143420568"/>
+        <c:axId val="2085989576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11572,7 +12016,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Additional cable length, km (worst case)</a:t>
+                  <a:t>Additional cost, thousands of EUROS (worst case)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -11585,12 +12029,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086101656"/>
+        <c:crossAx val="2145085528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2086101656"/>
+        <c:axId val="2145085528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11626,7 +12070,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2143420568"/>
+        <c:crossAx val="2085989576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11785,7 +12229,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overview!$E$5</c:f>
+              <c:f>Overview!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11796,7 +12240,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$G$7:$G$15</c:f>
+              <c:f>Overview!$H$7:$H$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11832,7 +12276,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overview!$E$7:$E$15</c:f>
+              <c:f>Overview!$F$7:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11873,7 +12317,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Overview!$H$5</c:f>
+              <c:f>Overview!$J$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11884,7 +12328,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$J$7:$J$15</c:f>
+              <c:f>Overview!$L$7:$L$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11920,7 +12364,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Overview!$H$7:$H$15</c:f>
+              <c:f>Overview!$J$7:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11964,11 +12408,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2142209176"/>
-        <c:axId val="2142663416"/>
+        <c:axId val="2086144280"/>
+        <c:axId val="2097938952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2142209176"/>
+        <c:axId val="2086144280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11999,12 +12443,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142663416"/>
+        <c:crossAx val="2097938952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2142663416"/>
+        <c:axId val="2097938952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12040,7 +12484,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2142209176"/>
+        <c:crossAx val="2086144280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12291,16 +12735,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12353,23 +12797,55 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0303_snap.20x3" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.20x3" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0203_snap.20x3" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_2" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0204_snap.20x3" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0208_snap.20x3" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0205_snap.20x3" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0207_snap.20x3" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12377,47 +12853,47 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0207_snap.20x3" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0205_snap.20x3" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0208_snap.20x3" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0204_snap.20x3" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_2" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0203_snap.20x3" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0300_snap.20x3" connectionId="17" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0202_snap.20x3" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.txt.20x3" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0302_snap.20x3" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.txt.20x3.txt.20x3" connectionId="25" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0200_snap.20x3" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0304_snap.20x3" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0301_snap.20x3" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_1" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0102_snap.20x3" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0108_snap.20x3" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0103_snap.20x3" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0107_snap.20x3" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0104_snap.20x3" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0106_snap.20x3" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12425,71 +12901,71 @@
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0106_snap.20x3" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0104_snap.20x3" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0107_snap.20x3" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0103_snap.20x3" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0108_snap.20x3" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0102_snap.20x3" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_1" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0200_snap.20x3" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.txt.20x3.txt.20x3" connectionId="25" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0306_snap.20x3" connectionId="23" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.20x3" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model01_cables" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model02_cables" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model03_cables" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1_v5_cables" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0305_snap.20x3" connectionId="22" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0302_snap.20x3" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1_v5_cables" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model03_cables" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model02_cables" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model01_cables" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0306_snap.20x3" connectionId="23" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0301_snap.20x3" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0201_snap.20x3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.20x3" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0304_snap.20x3" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.20x3" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0303_snap.20x3" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0201_snap.20x3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.txt.20x3" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0202_snap.20x3" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0300_snap.20x3" connectionId="17" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18979,10 +19455,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J41"/>
+  <dimension ref="A2:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I59" sqref="I59"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18996,23 +19472,23 @@
     <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:13">
       <c r="B2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:13">
       <c r="B4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>48</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -19022,20 +19498,20 @@
       <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>37</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -19046,22 +19522,34 @@
         <f>C40/1000</f>
         <v>6.6895706758067996</v>
       </c>
-      <c r="E6">
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <f>C40/1000</f>
         <v>6.6895706758067996</v>
       </c>
-      <c r="H6">
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <f>C40/1000</f>
         <v>6.6895706758067996</v>
       </c>
+      <c r="L6" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:13">
       <c r="A7">
         <v>0</v>
       </c>
@@ -19078,31 +19566,43 @@
         <v>4.6967467496540037E-3</v>
       </c>
       <c r="E7">
+        <f>C7*rfonfcost_per_station_per_km/1000</f>
+        <v>1.174186687413501</v>
+      </c>
+      <c r="F7">
         <f>'Snapshot setting'!F77</f>
         <v>0.89304880437868461</v>
       </c>
-      <c r="F7">
-        <f>(E30/1000)-F$6</f>
+      <c r="G7">
+        <f>(E30/1000)-G$6</f>
         <v>4.6472244574740005</v>
       </c>
-      <c r="G7">
-        <f>F7*1000/$C$41</f>
+      <c r="H7">
+        <f>G7*1000/$C$41</f>
         <v>1.8588897829896003E-2</v>
       </c>
-      <c r="H7">
+      <c r="I7">
+        <f>G7*rfonfcost_per_station_per_km/1000</f>
+        <v>4.6472244574740005</v>
+      </c>
+      <c r="J7">
         <f>'Snapshot setting'!F131</f>
         <v>0.89304880437868461</v>
       </c>
-      <c r="I7">
-        <f>(G30/1000)-I$6</f>
+      <c r="K7">
+        <f>(G30/1000)-K$6</f>
         <v>4.6472244574740005</v>
       </c>
-      <c r="J7">
-        <f>I7*1000/$C$41</f>
+      <c r="L7">
+        <f>K7*1000/$C$41</f>
         <v>1.8588897829896003E-2</v>
       </c>
+      <c r="M7">
+        <f>K7*rfonfcost_per_station_per_km/1000</f>
+        <v>4.6472244574740005</v>
+      </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:13">
       <c r="A8">
         <v>1</v>
       </c>
@@ -19111,7 +19611,7 @@
         <v>0.90192825074024086</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:E15" si="0">(C31/1000)-C$6</f>
+        <f t="shared" ref="C8:C15" si="0">(C31/1000)-C$6</f>
         <v>3.047565317308</v>
       </c>
       <c r="D8">
@@ -19119,31 +19619,43 @@
         <v>1.2190261269232E-2</v>
       </c>
       <c r="E8">
+        <f>C8*rfonfcost_per_station_per_km/1000</f>
+        <v>3.047565317308</v>
+      </c>
+      <c r="F8">
         <f>'Snapshot setting'!I77</f>
         <v>0.79273494051699289</v>
       </c>
-      <c r="F8">
-        <f>(E31/1000)-F$6</f>
+      <c r="G8">
+        <f>(E31/1000)-G$6</f>
         <v>11.358792842698499</v>
       </c>
-      <c r="G8">
-        <f t="shared" ref="G8:G15" si="2">F8*1000/$C$41</f>
+      <c r="H8">
+        <f t="shared" ref="H8:H15" si="2">G8*1000/$C$41</f>
         <v>4.5435171370793989E-2</v>
       </c>
-      <c r="H8">
+      <c r="I8">
+        <f>G8*rfonfcost_per_station_per_km/1000</f>
+        <v>11.358792842698499</v>
+      </c>
+      <c r="J8">
         <f>'Snapshot setting'!I131</f>
         <v>0.79273494051699289</v>
       </c>
-      <c r="I8">
-        <f>(G31/1000)-I$6</f>
+      <c r="K8">
+        <f>(G31/1000)-K$6</f>
         <v>11.358792842698499</v>
       </c>
-      <c r="J8">
-        <f t="shared" ref="J8:J15" si="3">I8*1000/$C$41</f>
+      <c r="L8">
+        <f t="shared" ref="L8:L15" si="3">K8*1000/$C$41</f>
         <v>4.5435171370793989E-2</v>
       </c>
+      <c r="M8">
+        <f>K8*rfonfcost_per_station_per_km/1000</f>
+        <v>11.358792842698499</v>
+      </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:13">
       <c r="A9">
         <v>2</v>
       </c>
@@ -19160,31 +19672,43 @@
         <v>2.3807854180272404E-2</v>
       </c>
       <c r="E9">
+        <f>C9*rfonfcost_per_station_per_km/1000</f>
+        <v>5.951963545068101</v>
+      </c>
+      <c r="F9">
         <f>'Snapshot setting'!L77</f>
         <v>0.71511632682091153</v>
       </c>
-      <c r="F9">
-        <f>(E32/1000)-F$6</f>
+      <c r="G9">
+        <f>(E32/1000)-G$6</f>
         <v>21.002906916146003</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <f t="shared" si="2"/>
         <v>8.4011627664584018E-2</v>
       </c>
-      <c r="H9">
+      <c r="I9">
+        <f>G9*rfonfcost_per_station_per_km/1000</f>
+        <v>21.002906916146003</v>
+      </c>
+      <c r="J9">
         <f>'Snapshot setting'!L131</f>
         <v>0.71511632682091153</v>
       </c>
-      <c r="I9">
-        <f>(G32/1000)-I$6</f>
+      <c r="K9">
+        <f>(G32/1000)-K$6</f>
         <v>21.002906916146003</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <f t="shared" si="3"/>
         <v>8.4011627664584018E-2</v>
       </c>
+      <c r="M9">
+        <f>K9*rfonfcost_per_station_per_km/1000</f>
+        <v>21.002906916146003</v>
+      </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>3</v>
       </c>
@@ -19201,31 +19725,43 @@
         <v>4.1179284723168404E-2</v>
       </c>
       <c r="E10">
+        <f>C10*rfonfcost_per_station_per_km/1000</f>
+        <v>10.294821180792102</v>
+      </c>
+      <c r="F10">
         <f>'Snapshot setting'!O77</f>
         <v>0.66534947072017703</v>
       </c>
-      <c r="F10">
-        <f>(E33/1000)-F$6</f>
+      <c r="G10">
+        <f>(E33/1000)-G$6</f>
         <v>34.7340257677076</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <f t="shared" si="2"/>
         <v>0.1389361030708304</v>
       </c>
-      <c r="H10">
+      <c r="I10">
+        <f>G10*rfonfcost_per_station_per_km/1000</f>
+        <v>34.7340257677076</v>
+      </c>
+      <c r="J10">
         <f>'Snapshot setting'!O131</f>
         <v>0.66534947072017703</v>
       </c>
-      <c r="I10">
-        <f>(G33/1000)-I$6</f>
+      <c r="K10">
+        <f>(G33/1000)-K$6</f>
         <v>34.7340257677076</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <f t="shared" si="3"/>
         <v>0.1389361030708304</v>
       </c>
+      <c r="M10">
+        <f>K10*rfonfcost_per_station_per_km/1000</f>
+        <v>34.7340257677076</v>
+      </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:13">
       <c r="A11">
         <v>4</v>
       </c>
@@ -19242,31 +19778,43 @@
         <v>6.1045867403431597E-2</v>
       </c>
       <c r="E11">
+        <f>C11*rfonfcost_per_station_per_km/1000</f>
+        <v>15.2614668508579</v>
+      </c>
+      <c r="F11">
         <f>'Snapshot setting'!R77</f>
         <v>0.61793507758333843</v>
       </c>
-      <c r="F11">
-        <f>(E34/1000)-F$6</f>
+      <c r="G11">
+        <f>(E34/1000)-G$6</f>
         <v>53.770356736764008</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <f t="shared" si="2"/>
         <v>0.21508142694705604</v>
       </c>
-      <c r="H11">
+      <c r="I11">
+        <f>G11*rfonfcost_per_station_per_km/1000</f>
+        <v>53.770356736764008</v>
+      </c>
+      <c r="J11">
         <f>'Snapshot setting'!R131</f>
         <v>0.61793507758333843</v>
       </c>
-      <c r="I11">
-        <f>(G34/1000)-I$6</f>
+      <c r="K11">
+        <f>(G34/1000)-K$6</f>
         <v>53.770356736764008</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <f t="shared" si="3"/>
         <v>0.21508142694705604</v>
       </c>
+      <c r="M11">
+        <f>K11*rfonfcost_per_station_per_km/1000</f>
+        <v>53.770356736764008</v>
+      </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:13">
       <c r="A12">
         <v>5</v>
       </c>
@@ -19283,31 +19831,43 @@
         <v>8.816631386824321E-2</v>
       </c>
       <c r="E12">
+        <f>C12*rfonfcost_per_station_per_km/1000</f>
+        <v>22.041578467060802</v>
+      </c>
+      <c r="F12">
         <f>'Snapshot setting'!U77</f>
         <v>0.5731765787721923</v>
       </c>
-      <c r="F12">
-        <f>(E35/1000)-F$6</f>
+      <c r="G12">
+        <f>(E35/1000)-G$6</f>
         <v>79.01679628508009</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <f t="shared" si="2"/>
         <v>0.31606718514032034</v>
       </c>
-      <c r="H12">
+      <c r="I12">
+        <f>G12*rfonfcost_per_station_per_km/1000</f>
+        <v>79.016796285080076</v>
+      </c>
+      <c r="J12">
         <f>'Snapshot setting'!U131</f>
         <v>0.55912287714994813</v>
       </c>
-      <c r="I12">
-        <f>(G35/1000)-I$6</f>
+      <c r="K12">
+        <f>(G35/1000)-K$6</f>
         <v>60.550468352966895</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <f t="shared" si="3"/>
         <v>0.24220187341186758</v>
       </c>
+      <c r="M12">
+        <f>K12*rfonfcost_per_station_per_km/1000</f>
+        <v>60.550468352966895</v>
+      </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:13">
       <c r="A13">
         <v>6</v>
       </c>
@@ -19324,31 +19884,43 @@
         <v>0.1245964609565616</v>
       </c>
       <c r="E13">
+        <f>C13*rfonfcost_per_station_per_km/1000</f>
+        <v>31.1491152391404</v>
+      </c>
+      <c r="F13">
         <f>'Snapshot setting'!X77</f>
         <v>0.51827031753603381</v>
       </c>
-      <c r="F13">
-        <f>(E36/1000)-F$6</f>
+      <c r="G13">
+        <f>(E36/1000)-G$6</f>
         <v>112.3569257895242</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <f t="shared" si="2"/>
         <v>0.44942770315809683</v>
       </c>
-      <c r="H13">
+      <c r="I13">
+        <f>G13*rfonfcost_per_station_per_km/1000</f>
+        <v>112.3569257895242</v>
+      </c>
+      <c r="J13">
         <f>'Snapshot setting'!X131</f>
         <v>0.50733798410346753</v>
       </c>
-      <c r="I13">
-        <f>(G36/1000)-I$6</f>
+      <c r="K13">
+        <f>(G36/1000)-K$6</f>
         <v>69.6580051250465</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <f t="shared" si="3"/>
         <v>0.27863202050018604</v>
       </c>
+      <c r="M13">
+        <f>K13*rfonfcost_per_station_per_km/1000</f>
+        <v>69.6580051250465</v>
+      </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:13">
       <c r="A14">
         <v>7</v>
       </c>
@@ -19365,31 +19937,43 @@
         <v>0.17320542756439042</v>
       </c>
       <c r="E14">
+        <f>C14*rfonfcost_per_station_per_km/1000</f>
+        <v>43.301356891097605</v>
+      </c>
+      <c r="F14">
         <f>'Snapshot setting'!AA77</f>
         <v>0.49565353657367195</v>
       </c>
-      <c r="F14">
-        <f>(E37/1000)-F$6</f>
+      <c r="G14">
+        <f>(E37/1000)-G$6</f>
         <v>156.30353403351319</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <f t="shared" si="2"/>
         <v>0.62521413613405274</v>
       </c>
-      <c r="H14">
+      <c r="I14">
+        <f>G14*rfonfcost_per_station_per_km/1000</f>
+        <v>156.30353403351319</v>
+      </c>
+      <c r="J14">
         <f>'Snapshot setting'!AA131</f>
         <v>0.47120530919363629</v>
       </c>
-      <c r="I14">
-        <f>(G37/1000)-I$6</f>
+      <c r="K14">
+        <f>(G37/1000)-K$6</f>
         <v>81.810246777003599</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <f t="shared" si="3"/>
         <v>0.32724098710801441</v>
       </c>
+      <c r="M14">
+        <f>K14*rfonfcost_per_station_per_km/1000</f>
+        <v>81.810246777003599</v>
+      </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:13">
       <c r="A15">
         <v>8</v>
       </c>
@@ -19406,28 +19990,50 @@
         <v>0.23905291648762678</v>
       </c>
       <c r="E15">
+        <f>C15*rfonfcost_per_station_per_km/1000</f>
+        <v>59.763229121906697</v>
+      </c>
+      <c r="F15">
         <f>'Snapshot setting'!AD77</f>
         <v>0.47932060504026291</v>
       </c>
-      <c r="F15">
-        <f>(E38/1000)-F$6</f>
+      <c r="G15">
+        <f>(E38/1000)-G$6</f>
         <v>214.47484712789219</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <f t="shared" si="2"/>
         <v>0.85789938851156877</v>
       </c>
-      <c r="H15">
+      <c r="I15">
+        <f>G15*rfonfcost_per_station_per_km/1000</f>
+        <v>214.47484712789219</v>
+      </c>
+      <c r="J15">
         <f>'Snapshot setting'!AD131</f>
         <v>0.42799534512599297</v>
       </c>
-      <c r="I15">
-        <f>(G38/1000)-I$6</f>
+      <c r="K15">
+        <f>(G38/1000)-K$6</f>
         <v>98.272119007812194</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <f t="shared" si="3"/>
         <v>0.39308847603124875</v>
+      </c>
+      <c r="M15">
+        <f>K15*rfonfcost_per_station_per_km/1000</f>
+        <v>98.272119007812194</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="H19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="H20" s="4">
+        <v>1000</v>
       </c>
     </row>
     <row r="28" spans="1:9">

</xml_diff>

<commit_message>
Removed spurios MST total, just use cost for extra cable now.
</commit_message>
<xml_diff>
--- a/results/iantconfig/Iantconfig_text_results/Antconfig_results_overview.xlsx
+++ b/results/iantconfig/Iantconfig_text_results/Antconfig_results_overview.xlsx
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="53">
   <si>
     <t>baseline</t>
   </si>
@@ -578,16 +578,7 @@
     <t>For inner array</t>
   </si>
   <si>
-    <t>V5 full array MST</t>
-  </si>
-  <si>
-    <t>Guess for now - need number</t>
-  </si>
-  <si>
     <t>RF on fibre cost per km per station</t>
-  </si>
-  <si>
-    <t>relative increase</t>
   </si>
   <si>
     <t>Cost increaes (kEUROS)</t>
@@ -664,8 +655,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -718,7 +711,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -741,6 +734,7 @@
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -763,6 +757,7 @@
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2386,11 +2381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2078347624"/>
-        <c:axId val="-2078600088"/>
+        <c:axId val="2142988344"/>
+        <c:axId val="2142752056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2078347624"/>
+        <c:axId val="2142988344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2403,12 +2398,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2078600088"/>
+        <c:crossAx val="2142752056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2078600088"/>
+        <c:axId val="2142752056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2422,427 +2417,13 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2078347624"/>
+        <c:crossAx val="2142988344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>UVGAP</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> ratio as function of cable length</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Overview!$B$6</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Overview!$C$7:$C$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>1.174186687413501</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.047565317308</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.9519635450681</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.2948211807921</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>15.2614668508579</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>22.0415784670608</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31.1491152391404</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43.3013568910976</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>59.7632291219067</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Overview!$B$7:$B$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.970887059894747</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.901928250740241</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.842262719639391</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.761651830255601</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.681377695741551</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.605407217034242</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.549089794972765</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.492312265095318</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.433705016363919</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Overview!$F$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Overview!$G$7:$G$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.647224457474</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.3587928426985</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.002906916146</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.7340257677076</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>53.770356736764</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>79.0167962850801</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>112.3569257895242</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>156.3035340335132</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>214.4748471278922</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Overview!$F$7:$F$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.893048804378685</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.792734940516993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.715116326820911</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.665349470720177</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.617935077583338</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.573176578772192</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.518270317536034</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.495653536573672</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.479320605040263</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Overview!$J$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Overview!$K$7:$K$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>4.647224457474</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>11.3587928426985</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.002906916146</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>34.7340257677076</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>53.770356736764</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>60.5504683529669</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>69.6580051250465</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>81.8102467770036</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>98.2721190078122</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Overview!$J$7:$J$15</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.893048804378685</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.792734940516993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.715116326820911</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.665349470720177</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.617935077583338</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.559122877149948</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.507337984103468</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.471205309193636</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.427995345125993</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2146145080"/>
-        <c:axId val="2146140328"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="2146145080"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Additional cable length, km (worst case)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146140328"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="2146140328"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:minorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>UVGAP</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> ratio</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2146145080"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4473,11 +4054,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2127323640"/>
-        <c:axId val="-2127068040"/>
+        <c:axId val="2094587016"/>
+        <c:axId val="-2123531272"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2127323640"/>
+        <c:axId val="2094587016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4490,12 +4071,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127068040"/>
+        <c:crossAx val="-2123531272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2127068040"/>
+        <c:axId val="-2123531272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4509,7 +4090,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2127323640"/>
+        <c:crossAx val="2094587016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6146,11 +5727,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2126261880"/>
-        <c:axId val="-2125481928"/>
+        <c:axId val="2140557704"/>
+        <c:axId val="-2129839944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2126261880"/>
+        <c:axId val="2140557704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,12 +5744,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2125481928"/>
+        <c:crossAx val="-2129839944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2125481928"/>
+        <c:axId val="-2129839944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6182,7 +5763,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126261880"/>
+        <c:crossAx val="2140557704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7819,11 +7400,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2126739880"/>
-        <c:axId val="-2126121112"/>
+        <c:axId val="2094197176"/>
+        <c:axId val="-2123754520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2126739880"/>
+        <c:axId val="2094197176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7836,12 +7417,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126121112"/>
+        <c:crossAx val="-2123754520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2126121112"/>
+        <c:axId val="-2123754520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7855,7 +7436,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126739880"/>
+        <c:crossAx val="2094197176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9492,11 +9073,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2104908968"/>
-        <c:axId val="-2081383448"/>
+        <c:axId val="2142580904"/>
+        <c:axId val="2141845480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2104908968"/>
+        <c:axId val="2142580904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9509,12 +9090,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2081383448"/>
+        <c:crossAx val="2141845480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2081383448"/>
+        <c:axId val="2141845480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9528,7 +9109,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2104908968"/>
+        <c:crossAx val="2142580904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11165,11 +10746,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085976472"/>
-        <c:axId val="2105173256"/>
+        <c:axId val="-2129880104"/>
+        <c:axId val="2142611208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085976472"/>
+        <c:axId val="-2129880104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11182,12 +10763,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105173256"/>
+        <c:crossAx val="2142611208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2105173256"/>
+        <c:axId val="2142611208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11201,7 +10782,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085976472"/>
+        <c:crossAx val="-2129880104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11578,11 +11159,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2099201960"/>
-        <c:axId val="2145322824"/>
+        <c:axId val="2142539160"/>
+        <c:axId val="2143106216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2099201960"/>
+        <c:axId val="2142539160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11616,12 +11197,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145322824"/>
+        <c:crossAx val="2143106216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145322824"/>
+        <c:axId val="2143106216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11656,7 +11237,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2099201960"/>
+        <c:crossAx val="2142539160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -11738,7 +11319,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$E$7:$E$15</c:f>
+              <c:f>Overview!$D$7:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -11994,11 +11575,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2085989576"/>
-        <c:axId val="2145085528"/>
+        <c:axId val="2140994312"/>
+        <c:axId val="-2129768920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2085989576"/>
+        <c:axId val="2140994312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12029,12 +11610,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2145085528"/>
+        <c:crossAx val="-2129768920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2145085528"/>
+        <c:axId val="-2129768920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12070,7 +11651,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085989576"/>
+        <c:crossAx val="2140994312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12152,36 +11733,36 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$D$7:$D$15</c:f>
+              <c:f>Overview!$C$7:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.004696746749654</c:v>
+                  <c:v>1.174186687413501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.012190261269232</c:v>
+                  <c:v>3.047565317308</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0238078541802724</c:v>
+                  <c:v>5.9519635450681</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0411792847231684</c:v>
+                  <c:v>10.2948211807921</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0610458674034316</c:v>
+                  <c:v>15.2614668508579</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0881663138682432</c:v>
+                  <c:v>22.0415784670608</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.124596460956562</c:v>
+                  <c:v>31.1491152391404</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.17320542756439</c:v>
+                  <c:v>43.3013568910976</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.239052916487627</c:v>
+                  <c:v>59.7632291219067</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12240,36 +11821,36 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$H$7:$H$15</c:f>
+              <c:f>Overview!$G$7:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.018588897829896</c:v>
+                  <c:v>4.647224457474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.045435171370794</c:v>
+                  <c:v>11.3587928426985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.084011627664584</c:v>
+                  <c:v>21.002906916146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13893610307083</c:v>
+                  <c:v>34.7340257677076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.215081426947056</c:v>
+                  <c:v>53.770356736764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.31606718514032</c:v>
+                  <c:v>79.0167962850801</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.449427703158097</c:v>
+                  <c:v>112.3569257895242</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.625214136134053</c:v>
+                  <c:v>156.3035340335132</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.857899388511569</c:v>
+                  <c:v>214.4748471278922</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12328,36 +11909,36 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Overview!$L$7:$L$15</c:f>
+              <c:f>Overview!$K$7:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.018588897829896</c:v>
+                  <c:v>4.647224457474</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.045435171370794</c:v>
+                  <c:v>11.3587928426985</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.084011627664584</c:v>
+                  <c:v>21.002906916146</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.13893610307083</c:v>
+                  <c:v>34.7340257677076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.215081426947056</c:v>
+                  <c:v>53.770356736764</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.242201873411868</c:v>
+                  <c:v>60.5504683529669</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.278632020500186</c:v>
+                  <c:v>69.6580051250465</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.327240987108014</c:v>
+                  <c:v>81.8102467770036</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.393088476031249</c:v>
+                  <c:v>98.2721190078122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12408,11 +11989,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2086144280"/>
-        <c:axId val="2097938952"/>
+        <c:axId val="-2130183336"/>
+        <c:axId val="2140195944"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2086144280"/>
+        <c:axId val="-2130183336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12430,7 +12011,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Additional cable length, as fraction of full array MST</a:t>
+                  <a:t>Additional cable length, km (worst case)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -12443,12 +12024,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097938952"/>
+        <c:crossAx val="2140195944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097938952"/>
+        <c:axId val="2140195944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12484,7 +12065,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086144280"/>
+        <c:crossAx val="-2130183336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12735,16 +12316,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12767,20 +12348,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -12797,55 +12378,23 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>81</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.20x3" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0304_snap.20x3" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_2" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0203_snap.20x3" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0208_snap.20x3" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0204_snap.20x3" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0207_snap.20x3" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0205_snap.20x3" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12853,47 +12402,47 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0205_snap.20x3" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0207_snap.20x3" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0204_snap.20x3" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0208_snap.20x3" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0203_snap.20x3" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_2" connectionId="34" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0202_snap.20x3" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0300_snap.20x3" connectionId="17" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0302_snap.20x3" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.20x3" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0200_snap.20x3" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.txt.20x3.txt.20x3" connectionId="25" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0301_snap.20x3" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0201_snap.20x3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_1" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0108_snap.20x3" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0102_snap.20x3" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0107_snap.20x3" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0103_snap.20x3" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0106_snap.20x3" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0104_snap.20x3" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12901,71 +12450,71 @@
 </file>
 
 <file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0104_snap.20x3" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0106_snap.20x3" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0103_snap.20x3" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0107_snap.20x3" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0102_snap.20x3" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0108_snap.20x3" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3" connectionId="32" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1v5_snap.20x3_1" connectionId="33" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.txt.20x3.txt.20x3" connectionId="25" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0200_snap.20x3" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0305_snap.20x3" connectionId="22" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0303_snap.20x3" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1_v5_cables" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model03_cables" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model02_cables" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model01_cables" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0306_snap.20x3" connectionId="23" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.20x3" connectionId="26" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model01_cables" connectionId="28" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model02_cables" connectionId="29" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="model03_cables" connectionId="30" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ska1_v5_cables" connectionId="31" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0305_snap.20x3" connectionId="22" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0201_snap.20x3" connectionId="9" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.txt.20x3" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0304_snap.20x3" connectionId="21" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0301_snap.20x3" connectionId="18" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0303_snap.20x3" connectionId="20" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0307_snap.20x3" connectionId="24" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0308_snap.txt.20x3" connectionId="27" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0302_snap.20x3" connectionId="19" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0300_snap.20x3" connectionId="17" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="0202_snap.20x3" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19455,10 +19004,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M41"/>
+  <dimension ref="A2:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K53" sqref="K53"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -19472,12 +19021,12 @@
     <col min="7" max="7" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:12">
       <c r="B2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:12">
       <c r="B4" t="s">
         <v>47</v>
       </c>
@@ -19488,7 +19037,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -19511,7 +19060,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -19523,10 +19072,7 @@
         <v>6.6895706758067996</v>
       </c>
       <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -19536,7 +19082,7 @@
         <v>6.6895706758067996</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -19546,10 +19092,10 @@
         <v>6.6895706758067996</v>
       </c>
       <c r="L6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>0</v>
       </c>
@@ -19562,10 +19108,6 @@
         <v>1.174186687413501</v>
       </c>
       <c r="D7">
-        <f>C7*1000/$C$41</f>
-        <v>4.6967467496540037E-3</v>
-      </c>
-      <c r="E7">
         <f>C7*rfonfcost_per_station_per_km/1000</f>
         <v>1.174186687413501</v>
       </c>
@@ -19574,14 +19116,10 @@
         <v>0.89304880437868461</v>
       </c>
       <c r="G7">
-        <f>(E30/1000)-G$6</f>
+        <f t="shared" ref="G7:G15" si="0">(E30/1000)-G$6</f>
         <v>4.6472244574740005</v>
       </c>
       <c r="H7">
-        <f>G7*1000/$C$41</f>
-        <v>1.8588897829896003E-2</v>
-      </c>
-      <c r="I7">
         <f>G7*rfonfcost_per_station_per_km/1000</f>
         <v>4.6472244574740005</v>
       </c>
@@ -19590,19 +19128,15 @@
         <v>0.89304880437868461</v>
       </c>
       <c r="K7">
-        <f>(G30/1000)-K$6</f>
+        <f t="shared" ref="K7:K15" si="1">(G30/1000)-K$6</f>
         <v>4.6472244574740005</v>
       </c>
       <c r="L7">
-        <f>K7*1000/$C$41</f>
-        <v>1.8588897829896003E-2</v>
-      </c>
-      <c r="M7">
         <f>K7*rfonfcost_per_station_per_km/1000</f>
         <v>4.6472244574740005</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1</v>
       </c>
@@ -19611,14 +19145,10 @@
         <v>0.90192825074024086</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C15" si="0">(C31/1000)-C$6</f>
+        <f t="shared" ref="C8:C15" si="2">(C31/1000)-C$6</f>
         <v>3.047565317308</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D15" si="1">C8*1000/$C$41</f>
-        <v>1.2190261269232E-2</v>
-      </c>
-      <c r="E8">
         <f>C8*rfonfcost_per_station_per_km/1000</f>
         <v>3.047565317308</v>
       </c>
@@ -19627,14 +19157,10 @@
         <v>0.79273494051699289</v>
       </c>
       <c r="G8">
-        <f>(E31/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>11.358792842698499</v>
       </c>
       <c r="H8">
-        <f t="shared" ref="H8:H15" si="2">G8*1000/$C$41</f>
-        <v>4.5435171370793989E-2</v>
-      </c>
-      <c r="I8">
         <f>G8*rfonfcost_per_station_per_km/1000</f>
         <v>11.358792842698499</v>
       </c>
@@ -19643,19 +19169,15 @@
         <v>0.79273494051699289</v>
       </c>
       <c r="K8">
-        <f>(G31/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>11.358792842698499</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L15" si="3">K8*1000/$C$41</f>
-        <v>4.5435171370793989E-2</v>
-      </c>
-      <c r="M8">
         <f>K8*rfonfcost_per_station_per_km/1000</f>
         <v>11.358792842698499</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2</v>
       </c>
@@ -19664,14 +19186,10 @@
         <v>0.84226271963939114</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>5.951963545068101</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>2.3807854180272404E-2</v>
-      </c>
-      <c r="E9">
         <f>C9*rfonfcost_per_station_per_km/1000</f>
         <v>5.951963545068101</v>
       </c>
@@ -19680,14 +19198,10 @@
         <v>0.71511632682091153</v>
       </c>
       <c r="G9">
-        <f>(E32/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>21.002906916146003</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
-        <v>8.4011627664584018E-2</v>
-      </c>
-      <c r="I9">
         <f>G9*rfonfcost_per_station_per_km/1000</f>
         <v>21.002906916146003</v>
       </c>
@@ -19696,19 +19210,15 @@
         <v>0.71511632682091153</v>
       </c>
       <c r="K9">
-        <f>(G32/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>21.002906916146003</v>
       </c>
       <c r="L9">
-        <f t="shared" si="3"/>
-        <v>8.4011627664584018E-2</v>
-      </c>
-      <c r="M9">
         <f>K9*rfonfcost_per_station_per_km/1000</f>
         <v>21.002906916146003</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>3</v>
       </c>
@@ -19717,14 +19227,10 @@
         <v>0.7616518302556009</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10.294821180792102</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>4.1179284723168404E-2</v>
-      </c>
-      <c r="E10">
         <f>C10*rfonfcost_per_station_per_km/1000</f>
         <v>10.294821180792102</v>
       </c>
@@ -19733,14 +19239,10 @@
         <v>0.66534947072017703</v>
       </c>
       <c r="G10">
-        <f>(E33/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>34.7340257677076</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
-        <v>0.1389361030708304</v>
-      </c>
-      <c r="I10">
         <f>G10*rfonfcost_per_station_per_km/1000</f>
         <v>34.7340257677076</v>
       </c>
@@ -19749,19 +19251,15 @@
         <v>0.66534947072017703</v>
       </c>
       <c r="K10">
-        <f>(G33/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>34.7340257677076</v>
       </c>
       <c r="L10">
-        <f t="shared" si="3"/>
-        <v>0.1389361030708304</v>
-      </c>
-      <c r="M10">
         <f>K10*rfonfcost_per_station_per_km/1000</f>
         <v>34.7340257677076</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>4</v>
       </c>
@@ -19770,14 +19268,10 @@
         <v>0.68137769574155072</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>15.2614668508579</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>6.1045867403431597E-2</v>
-      </c>
-      <c r="E11">
         <f>C11*rfonfcost_per_station_per_km/1000</f>
         <v>15.2614668508579</v>
       </c>
@@ -19786,14 +19280,10 @@
         <v>0.61793507758333843</v>
       </c>
       <c r="G11">
-        <f>(E34/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>53.770356736764008</v>
       </c>
       <c r="H11">
-        <f t="shared" si="2"/>
-        <v>0.21508142694705604</v>
-      </c>
-      <c r="I11">
         <f>G11*rfonfcost_per_station_per_km/1000</f>
         <v>53.770356736764008</v>
       </c>
@@ -19802,19 +19292,15 @@
         <v>0.61793507758333843</v>
       </c>
       <c r="K11">
-        <f>(G34/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>53.770356736764008</v>
       </c>
       <c r="L11">
-        <f t="shared" si="3"/>
-        <v>0.21508142694705604</v>
-      </c>
-      <c r="M11">
         <f>K11*rfonfcost_per_station_per_km/1000</f>
         <v>53.770356736764008</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>5</v>
       </c>
@@ -19823,14 +19309,10 @@
         <v>0.60540721703424183</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>22.041578467060802</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
-        <v>8.816631386824321E-2</v>
-      </c>
-      <c r="E12">
         <f>C12*rfonfcost_per_station_per_km/1000</f>
         <v>22.041578467060802</v>
       </c>
@@ -19839,14 +19321,10 @@
         <v>0.5731765787721923</v>
       </c>
       <c r="G12">
-        <f>(E35/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>79.01679628508009</v>
       </c>
       <c r="H12">
-        <f t="shared" si="2"/>
-        <v>0.31606718514032034</v>
-      </c>
-      <c r="I12">
         <f>G12*rfonfcost_per_station_per_km/1000</f>
         <v>79.016796285080076</v>
       </c>
@@ -19855,19 +19333,15 @@
         <v>0.55912287714994813</v>
       </c>
       <c r="K12">
-        <f>(G35/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>60.550468352966895</v>
       </c>
       <c r="L12">
-        <f t="shared" si="3"/>
-        <v>0.24220187341186758</v>
-      </c>
-      <c r="M12">
         <f>K12*rfonfcost_per_station_per_km/1000</f>
         <v>60.550468352966895</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>6</v>
       </c>
@@ -19876,14 +19350,10 @@
         <v>0.54908979497276533</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>31.1491152391404</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
-        <v>0.1245964609565616</v>
-      </c>
-      <c r="E13">
         <f>C13*rfonfcost_per_station_per_km/1000</f>
         <v>31.1491152391404</v>
       </c>
@@ -19892,14 +19362,10 @@
         <v>0.51827031753603381</v>
       </c>
       <c r="G13">
-        <f>(E36/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>112.3569257895242</v>
       </c>
       <c r="H13">
-        <f t="shared" si="2"/>
-        <v>0.44942770315809683</v>
-      </c>
-      <c r="I13">
         <f>G13*rfonfcost_per_station_per_km/1000</f>
         <v>112.3569257895242</v>
       </c>
@@ -19908,19 +19374,15 @@
         <v>0.50733798410346753</v>
       </c>
       <c r="K13">
-        <f>(G36/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>69.6580051250465</v>
       </c>
       <c r="L13">
-        <f t="shared" si="3"/>
-        <v>0.27863202050018604</v>
-      </c>
-      <c r="M13">
         <f>K13*rfonfcost_per_station_per_km/1000</f>
         <v>69.6580051250465</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>7</v>
       </c>
@@ -19929,14 +19391,10 @@
         <v>0.49231226509531784</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43.301356891097605</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
-        <v>0.17320542756439042</v>
-      </c>
-      <c r="E14">
         <f>C14*rfonfcost_per_station_per_km/1000</f>
         <v>43.301356891097605</v>
       </c>
@@ -19945,14 +19403,10 @@
         <v>0.49565353657367195</v>
       </c>
       <c r="G14">
-        <f>(E37/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>156.30353403351319</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
-        <v>0.62521413613405274</v>
-      </c>
-      <c r="I14">
         <f>G14*rfonfcost_per_station_per_km/1000</f>
         <v>156.30353403351319</v>
       </c>
@@ -19961,19 +19415,15 @@
         <v>0.47120530919363629</v>
       </c>
       <c r="K14">
-        <f>(G37/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>81.810246777003599</v>
       </c>
       <c r="L14">
-        <f t="shared" si="3"/>
-        <v>0.32724098710801441</v>
-      </c>
-      <c r="M14">
         <f>K14*rfonfcost_per_station_per_km/1000</f>
         <v>81.810246777003599</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>8</v>
       </c>
@@ -19982,14 +19432,10 @@
         <v>0.43370501636391867</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>59.763229121906697</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>0.23905291648762678</v>
-      </c>
-      <c r="E15">
         <f>C15*rfonfcost_per_station_per_km/1000</f>
         <v>59.763229121906697</v>
       </c>
@@ -19998,14 +19444,10 @@
         <v>0.47932060504026291</v>
       </c>
       <c r="G15">
-        <f>(E38/1000)-G$6</f>
+        <f t="shared" si="0"/>
         <v>214.47484712789219</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
-        <v>0.85789938851156877</v>
-      </c>
-      <c r="I15">
         <f>G15*rfonfcost_per_station_per_km/1000</f>
         <v>214.47484712789219</v>
       </c>
@@ -20014,21 +19456,17 @@
         <v>0.42799534512599297</v>
       </c>
       <c r="K15">
-        <f>(G38/1000)-K$6</f>
+        <f t="shared" si="1"/>
         <v>98.272119007812194</v>
       </c>
       <c r="L15">
-        <f t="shared" si="3"/>
-        <v>0.39308847603124875</v>
-      </c>
-      <c r="M15">
         <f>K15*rfonfcost_per_station_per_km/1000</f>
         <v>98.272119007812194</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="H19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -20292,18 +19730,8 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>51</v>
-      </c>
-      <c r="B41" s="2">
-        <v>0</v>
-      </c>
-      <c r="C41" s="2">
-        <v>250000</v>
-      </c>
-      <c r="D41" t="s">
-        <v>52</v>
-      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>